<commit_message>
payables receivables are seperated,other changes are also done
</commit_message>
<xml_diff>
--- a/public/reports/accounts_report_g.xlsx
+++ b/public/reports/accounts_report_g.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="64">
   <si>
     <t>ACCOUNTS REPORT</t>
   </si>
@@ -22,7 +22,7 @@
     <t>Generated on</t>
   </si>
   <si>
-    <t>17/1/2019</t>
+    <t>22/1/2019</t>
   </si>
   <si>
     <t>Accounts Recievables</t>
@@ -64,25 +64,40 @@
     <t>lpo/Dream uniforms/12369</t>
   </si>
   <si>
+    <t>59640</t>
+  </si>
+  <si>
+    <t>2019-01-19</t>
+  </si>
+  <si>
+    <t>75000.00</t>
+  </si>
+  <si>
+    <t>fayyaz threading co</t>
+  </si>
+  <si>
+    <t>po/fayyaz threading co/2019/3</t>
+  </si>
+  <si>
+    <t>33443</t>
+  </si>
+  <si>
+    <t>2019-01-11</t>
+  </si>
+  <si>
+    <t>74900</t>
+  </si>
+  <si>
     <t>27429</t>
   </si>
   <si>
-    <t>2019-01-11</t>
-  </si>
-  <si>
     <t>0.00</t>
   </si>
   <si>
-    <t>fayyaz threading co</t>
-  </si>
-  <si>
-    <t>po/fayyaz threading co/2019/3</t>
-  </si>
-  <si>
-    <t>33443</t>
-  </si>
-  <si>
-    <t>74900</t>
+    <t>8787878</t>
+  </si>
+  <si>
+    <t>74150</t>
   </si>
   <si>
     <t>lpo/Dream uniforms/65662</t>
@@ -94,46 +109,103 @@
     <t>2019-01-12</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t>95920</t>
+  </si>
+  <si>
+    <t>37500</t>
+  </si>
+  <si>
+    <t>lpo/Dream uniforms/78605</t>
+  </si>
+  <si>
+    <t>52003</t>
+  </si>
+  <si>
+    <t>34343</t>
+  </si>
+  <si>
+    <t>2019-01-18</t>
+  </si>
+  <si>
+    <t>37400</t>
+  </si>
+  <si>
+    <t>Affan uniforms co.</t>
+  </si>
+  <si>
+    <t>lpo/Affan uniforms co./500</t>
+  </si>
+  <si>
+    <t>2019/1</t>
+  </si>
+  <si>
+    <t>2019-01-14</t>
+  </si>
+  <si>
+    <t>15000.00</t>
+  </si>
+  <si>
+    <t>Abbas Ali and sons</t>
+  </si>
+  <si>
+    <t>po/Abbas Ali and sons/2019/7</t>
+  </si>
+  <si>
+    <t>2019/200</t>
+  </si>
+  <si>
+    <t>2019-01-24</t>
+  </si>
+  <si>
+    <t>7500</t>
+  </si>
+  <si>
+    <t>2019/2</t>
+  </si>
+  <si>
+    <t>2019-01-15</t>
+  </si>
+  <si>
+    <t>5100.00</t>
+  </si>
+  <si>
+    <t>po/Abbas Ali and sons/2019/8</t>
+  </si>
+  <si>
+    <t>231</t>
+  </si>
+  <si>
+    <t>80000</t>
+  </si>
+  <si>
+    <t>lpo/Dream uniforms/73315</t>
+  </si>
+  <si>
+    <t>2019/3</t>
+  </si>
+  <si>
+    <t>37200.00</t>
+  </si>
+  <si>
+    <t>2019/4</t>
+  </si>
+  <si>
+    <t>28500.00</t>
+  </si>
+  <si>
     <t>Total Payables</t>
   </si>
   <si>
-    <t>74900.00</t>
-  </si>
-  <si>
-    <t>lpo/Dream uniforms/78605</t>
-  </si>
-  <si>
-    <t>52003</t>
-  </si>
-  <si>
-    <t>Affan uniforms co.</t>
-  </si>
-  <si>
-    <t>lpo/Affan uniforms co./500</t>
-  </si>
-  <si>
-    <t>2019/1</t>
-  </si>
-  <si>
-    <t>2019-01-14</t>
-  </si>
-  <si>
-    <t>15000.00</t>
-  </si>
-  <si>
-    <t>2019/2</t>
-  </si>
-  <si>
-    <t>2019-01-15</t>
-  </si>
-  <si>
-    <t>5100.00</t>
+    <t>386350.00</t>
   </si>
   <si>
     <t>Total Recievables</t>
   </si>
   <si>
-    <t>20100.00</t>
+    <t>160800.00</t>
   </si>
 </sst>
 </file>
@@ -478,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="H11" sqref="H11"/>
@@ -606,10 +678,10 @@
         <v>21</v>
       </c>
       <c r="K6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="L6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -620,25 +692,37 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
         <v>24</v>
       </c>
       <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
         <v>25</v>
       </c>
-      <c r="F7" t="s">
-        <v>18</v>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" t="s">
+        <v>26</v>
       </c>
       <c r="K7" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="L7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -652,58 +736,234 @@
         <v>29</v>
       </c>
       <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
         <v>25</v>
       </c>
-      <c r="F8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
         <v>32</v>
       </c>
       <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" t="s">
         <v>33</v>
       </c>
-      <c r="F9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
         <v>35</v>
       </c>
       <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" t="s">
         <v>36</v>
       </c>
-      <c r="F10" t="s">
+      <c r="K10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11">
+        <v>6</v>
+      </c>
+      <c r="H11" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" t="s">
+        <v>46</v>
+      </c>
+      <c r="K11" t="s">
+        <v>47</v>
+      </c>
+      <c r="L11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
         <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12">
+        <v>7</v>
+      </c>
+      <c r="H12" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" t="s">
+        <v>52</v>
+      </c>
+      <c r="J12" t="s">
+        <v>53</v>
+      </c>
+      <c r="K12" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" t="s">
+        <v>59</v>
+      </c>
+      <c r="K14" t="s">
+        <v>60</v>
+      </c>
+      <c r="L14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>